<commit_message>
Added cmip6 mappings for cmip5-atmos-key-properties.xlsx
</commit_message>
<xml_diff>
--- a/mappings/cmip5-atmos-key-properties.xlsx
+++ b/mappings/cmip5-atmos-key-properties.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
-  <workbookPr date1904="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/cmip6/cmip6-specializations-atmos/mappings/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="30100" yWindow="0" windowWidth="19240" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>cmip5-component-property</t>
   </si>
@@ -105,13 +100,40 @@
   </si>
   <si>
     <t>cmip6.atmos.key_properties.orography.type</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.insolation_ozone.solar_ozone_impact</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.orbital_parameters.computation_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.orbital_parameters.fixed_reference_date</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.orbital_parameters.solar_constant_transient_characteristics</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.orbital_parameters.type</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.solar_constant.type</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.solar_constant.transient_characteristics</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.solar.solar_constant.fixed_value</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.volcanos.volcanoes_treatment.volcanoes_implementation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -126,6 +148,23 @@
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Helvetica"/>
     </font>
   </fonts>
@@ -143,7 +182,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -196,13 +235,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA5A5A5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA5A5A5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA5A5A5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5A5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -221,8 +341,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="23">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1413,21 +1558,21 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="78.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="55.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="91.6640625" style="1" customWidth="1"/>
     <col min="3" max="254" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="28" customHeight="1">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
     </row>
-    <row r="2" spans="1:2" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="20.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1435,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="20.25" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1443,19 +1588,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="20.25" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="20.25" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="20.25" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1463,121 +1608,143 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="20.25" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="20.25" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="20.25" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20.25" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="20.25" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="20.25" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="20.25" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" ht="20.25" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" ht="20.25" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="20.25" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="20.25" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="20.25" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" ht="20.25" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2" ht="20.25" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="20.25" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="20.25" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="20.25" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="20.25" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2" ht="20.25" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="20.25" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2" ht="20.25" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
@@ -1592,5 +1759,10 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>